<commit_message>
fix error on goods management
</commit_message>
<xml_diff>
--- a/assets/format/template_master.xlsx
+++ b/assets/format/template_master.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\sgss-web\assets\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864576B9-F2FB-4BA7-BE6E-07DE93D1A609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517F510F-0522-4A24-8ECC-4BA8C6BD828A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{2F15F523-A8F8-4B01-A65B-6B4F5ED804C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="6" xr2:uid="{2F15F523-A8F8-4B01-A65B-6B4F5ED804C2}"/>
   </bookViews>
   <sheets>
     <sheet name="UoM" sheetId="1" r:id="rId1"/>
     <sheet name="Category" sheetId="2" r:id="rId2"/>
     <sheet name="Factory" sheetId="3" r:id="rId3"/>
     <sheet name="Item Group" sheetId="7" r:id="rId4"/>
-    <sheet name="Master Material" sheetId="4" r:id="rId5"/>
+    <sheet name="Master Item" sheetId="4" r:id="rId5"/>
     <sheet name="Master Vendor" sheetId="5" r:id="rId6"/>
-    <sheet name="Master Vendor x Material" sheetId="6" r:id="rId7"/>
+    <sheet name="Master Vendor x Item" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -656,12 +656,12 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="23.77734375" style="1" customWidth="1"/>
+    <col min="1" max="2" width="23.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -669,159 +669,159 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
     </row>
@@ -836,131 +836,131 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
     </row>
   </sheetData>
@@ -974,131 +974,131 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
     </row>
   </sheetData>
@@ -1112,131 +1112,131 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
     </row>
   </sheetData>
@@ -1252,13 +1252,13 @@
       <selection sqref="A1:Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="15" style="1" customWidth="1"/>
     <col min="9" max="26" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>30</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1400,7 +1400,7 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1428,7 +1428,7 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1456,7 +1456,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1484,7 +1484,7 @@
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1512,7 +1512,7 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1540,7 +1540,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1568,7 +1568,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1596,7 +1596,7 @@
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1624,7 +1624,7 @@
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1652,7 +1652,7 @@
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1680,7 +1680,7 @@
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1708,7 +1708,7 @@
       <c r="Y14" s="5"/>
       <c r="Z14" s="5"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1736,7 +1736,7 @@
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1764,7 +1764,7 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1792,7 +1792,7 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1820,7 +1820,7 @@
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1848,7 +1848,7 @@
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1876,7 +1876,7 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1904,7 +1904,7 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1932,7 +1932,7 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1960,7 +1960,7 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1988,7 +1988,7 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2016,7 +2016,7 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2044,7 +2044,7 @@
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2072,7 +2072,7 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2100,7 +2100,7 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2128,7 +2128,7 @@
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2156,7 +2156,7 @@
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2184,7 +2184,7 @@
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2212,7 +2212,7 @@
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2240,7 +2240,7 @@
       <c r="Y33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2268,7 +2268,7 @@
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2296,7 +2296,7 @@
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2324,7 +2324,7 @@
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2352,7 +2352,7 @@
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2380,7 +2380,7 @@
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2408,7 +2408,7 @@
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2436,7 +2436,7 @@
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2464,7 +2464,7 @@
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2492,7 +2492,7 @@
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2520,7 +2520,7 @@
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2548,7 +2548,7 @@
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2576,7 +2576,7 @@
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2604,7 +2604,7 @@
       <c r="Y46" s="5"/>
       <c r="Z46" s="5"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2632,7 +2632,7 @@
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2660,7 +2660,7 @@
       <c r="Y48" s="5"/>
       <c r="Z48" s="5"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2688,7 +2688,7 @@
       <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2716,7 +2716,7 @@
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2744,7 +2744,7 @@
       <c r="Y51" s="5"/>
       <c r="Z51" s="5"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2772,7 +2772,7 @@
       <c r="Y52" s="5"/>
       <c r="Z52" s="5"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2800,7 +2800,7 @@
       <c r="Y53" s="5"/>
       <c r="Z53" s="5"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2828,7 +2828,7 @@
       <c r="Y54" s="5"/>
       <c r="Z54" s="5"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2856,7 +2856,7 @@
       <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2884,7 +2884,7 @@
       <c r="Y56" s="5"/>
       <c r="Z56" s="5"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2912,7 +2912,7 @@
       <c r="Y57" s="5"/>
       <c r="Z57" s="5"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2940,7 +2940,7 @@
       <c r="Y58" s="5"/>
       <c r="Z58" s="5"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2968,7 +2968,7 @@
       <c r="Y59" s="5"/>
       <c r="Z59" s="5"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2996,7 +2996,7 @@
       <c r="Y60" s="5"/>
       <c r="Z60" s="5"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3024,7 +3024,7 @@
       <c r="Y61" s="5"/>
       <c r="Z61" s="5"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -3052,7 +3052,7 @@
       <c r="Y62" s="5"/>
       <c r="Z62" s="5"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -3080,7 +3080,7 @@
       <c r="Y63" s="5"/>
       <c r="Z63" s="5"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3108,7 +3108,7 @@
       <c r="Y64" s="5"/>
       <c r="Z64" s="5"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -3136,7 +3136,7 @@
       <c r="Y65" s="5"/>
       <c r="Z65" s="5"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -3164,7 +3164,7 @@
       <c r="Y66" s="5"/>
       <c r="Z66" s="5"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3192,7 +3192,7 @@
       <c r="Y67" s="5"/>
       <c r="Z67" s="5"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3220,7 +3220,7 @@
       <c r="Y68" s="5"/>
       <c r="Z68" s="5"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3248,7 +3248,7 @@
       <c r="Y69" s="5"/>
       <c r="Z69" s="5"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3276,7 +3276,7 @@
       <c r="Y70" s="5"/>
       <c r="Z70" s="5"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -3304,7 +3304,7 @@
       <c r="Y71" s="5"/>
       <c r="Z71" s="5"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -3332,7 +3332,7 @@
       <c r="Y72" s="5"/>
       <c r="Z72" s="5"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -3360,7 +3360,7 @@
       <c r="Y73" s="5"/>
       <c r="Z73" s="5"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -3388,7 +3388,7 @@
       <c r="Y74" s="5"/>
       <c r="Z74" s="5"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -3416,7 +3416,7 @@
       <c r="Y75" s="5"/>
       <c r="Z75" s="5"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -3444,7 +3444,7 @@
       <c r="Y76" s="5"/>
       <c r="Z76" s="5"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -3472,7 +3472,7 @@
       <c r="Y77" s="5"/>
       <c r="Z77" s="5"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -3500,7 +3500,7 @@
       <c r="Y78" s="5"/>
       <c r="Z78" s="5"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -3528,7 +3528,7 @@
       <c r="Y79" s="5"/>
       <c r="Z79" s="5"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -3556,7 +3556,7 @@
       <c r="Y80" s="5"/>
       <c r="Z80" s="5"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -3584,7 +3584,7 @@
       <c r="Y81" s="5"/>
       <c r="Z81" s="5"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -3631,13 +3631,13 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="25.109375" style="1" customWidth="1"/>
-    <col min="6" max="11" width="25.109375" customWidth="1"/>
+    <col min="1" max="5" width="25.140625" style="1" customWidth="1"/>
+    <col min="6" max="11" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3685,7 +3685,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3698,7 +3698,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3711,7 +3711,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -3724,7 +3724,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -3737,7 +3737,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3750,7 +3750,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3763,7 +3763,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3776,7 +3776,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3789,7 +3789,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -3802,7 +3802,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -3815,7 +3815,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -3828,7 +3828,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -3841,7 +3841,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -3854,7 +3854,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -3867,7 +3867,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -3880,7 +3880,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3893,7 +3893,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -3906,7 +3906,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3919,7 +3919,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -3932,7 +3932,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3945,7 +3945,7 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3958,7 +3958,7 @@
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -3971,7 +3971,7 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3984,7 +3984,7 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3997,7 +3997,7 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -4010,7 +4010,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -4023,7 +4023,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -4036,7 +4036,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -4049,7 +4049,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -4062,7 +4062,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -4075,7 +4075,7 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -4088,7 +4088,7 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -4101,7 +4101,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -4114,7 +4114,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -4127,7 +4127,7 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -4140,7 +4140,7 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -4153,7 +4153,7 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -4166,7 +4166,7 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -4189,26 +4189,26 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
-    <col min="3" max="5" width="19.6640625" style="1" customWidth="1"/>
-    <col min="6" max="9" width="19.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="5" width="19.7109375" style="1" customWidth="1"/>
+    <col min="6" max="9" width="19.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="6"/>
       <c r="C2" s="4"/>
@@ -4280,7 +4280,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="6"/>
       <c r="C3" s="4"/>
@@ -4299,7 +4299,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="6"/>
       <c r="C4" s="4"/>
@@ -4318,7 +4318,7 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="6"/>
       <c r="C5" s="4"/>
@@ -4337,7 +4337,7 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="4"/>
@@ -4356,7 +4356,7 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
@@ -4375,7 +4375,7 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
@@ -4394,7 +4394,7 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
@@ -4413,7 +4413,7 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
@@ -4432,7 +4432,7 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
@@ -4451,7 +4451,7 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
@@ -4470,7 +4470,7 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="4"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
@@ -4489,7 +4489,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
@@ -4508,7 +4508,7 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
@@ -4527,7 +4527,7 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="4"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
@@ -4546,7 +4546,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
@@ -4565,7 +4565,7 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="4"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
@@ -4584,7 +4584,7 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
@@ -4603,7 +4603,7 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
@@ -4622,7 +4622,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="4"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
@@ -4641,7 +4641,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
@@ -4660,7 +4660,7 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
@@ -4679,7 +4679,7 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6"/>
       <c r="C24" s="4"/>
@@ -4698,7 +4698,7 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="4"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6"/>
       <c r="C25" s="4"/>
@@ -4717,7 +4717,7 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="4"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6"/>
       <c r="C26" s="4"/>
@@ -4736,7 +4736,7 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="4"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="6"/>
       <c r="C27" s="4"/>
@@ -4755,7 +4755,7 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="4"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6"/>
       <c r="C28" s="4"/>
@@ -4774,7 +4774,7 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="4"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6"/>
       <c r="C29" s="4"/>
@@ -4793,7 +4793,7 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="4"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6"/>
       <c r="C30" s="4"/>
@@ -4812,7 +4812,7 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="4"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6"/>
       <c r="C31" s="4"/>
@@ -4831,7 +4831,7 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="4"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6"/>
       <c r="C32" s="4"/>
@@ -4850,7 +4850,7 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="4"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6"/>
       <c r="C33" s="4"/>
@@ -4869,7 +4869,7 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="4"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6"/>
       <c r="C34" s="4"/>
@@ -4888,7 +4888,7 @@
       <c r="P34" s="7"/>
       <c r="Q34" s="4"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="6"/>
       <c r="C35" s="4"/>
@@ -4907,7 +4907,7 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="4"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="6"/>
       <c r="C36" s="4"/>
@@ -4926,7 +4926,7 @@
       <c r="P36" s="7"/>
       <c r="Q36" s="4"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6"/>
       <c r="C37" s="4"/>
@@ -4945,7 +4945,7 @@
       <c r="P37" s="7"/>
       <c r="Q37" s="4"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="6"/>
       <c r="C38" s="4"/>
@@ -4964,7 +4964,7 @@
       <c r="P38" s="7"/>
       <c r="Q38" s="4"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="6"/>
       <c r="C39" s="4"/>
@@ -4983,7 +4983,7 @@
       <c r="P39" s="7"/>
       <c r="Q39" s="4"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="6"/>
       <c r="C40" s="4"/>

</xml_diff>